<commit_message>
Feature: Updated image paths and added zoom/pan functionality to D3 tree.
</commit_message>
<xml_diff>
--- a/data/family_data.xlsx
+++ b/data/family_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savch\Google Drive\Work\Family-tree_v6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savch\Google Drive\Work\Family-tree_v6\web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DAFEC5-92B9-41A0-87C0-14A6F7AD6F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673C019D-DD51-4F97-891F-0BEF7E8137FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="18270" windowHeight="12930" xr2:uid="{856ECC72-5591-4C4C-B766-66B52D7AE0AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17880" windowHeight="15600" xr2:uid="{856ECC72-5591-4C4C-B766-66B52D7AE0AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="200">
   <si>
     <t>PersonID</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Science, engineering</t>
   </si>
   <si>
-    <t>leonid.png</t>
-  </si>
-  <si>
     <t>Elena</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Teaching</t>
   </si>
   <si>
-    <t>elena.png</t>
-  </si>
-  <si>
     <t>Sergey</t>
   </si>
   <si>
@@ -141,9 +135,6 @@
     <t>Sankt-Peterburg, Russia</t>
   </si>
   <si>
-    <t>sergey.png</t>
-  </si>
-  <si>
     <t>Dima</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>Villach, Austria</t>
   </si>
   <si>
-    <t>ms.png</t>
-  </si>
-  <si>
     <t>Sophia</t>
   </si>
   <si>
@@ -189,9 +177,6 @@
     <t>Homemaker</t>
   </si>
   <si>
-    <t>sophia.png</t>
-  </si>
-  <si>
     <t>Sviatik</t>
   </si>
   <si>
@@ -243,9 +228,6 @@
     <t>15.01.1947</t>
   </si>
   <si>
-    <t>milana.png</t>
-  </si>
-  <si>
     <t>Gleb</t>
   </si>
   <si>
@@ -478,19 +460,189 @@
   </si>
   <si>
     <t>Евгений</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>3, 4, 5</t>
+  </si>
+  <si>
+    <t>4, 5</t>
+  </si>
+  <si>
+    <t>3, 5</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>12, 13</t>
+  </si>
+  <si>
+    <t>6, 8</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>16, 17</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>25, 26</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>29, 33, 34, 35</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>39, 40, 41</t>
+  </si>
+  <si>
+    <t>45, 46</t>
+  </si>
+  <si>
+    <t>54, 55</t>
+  </si>
+  <si>
+    <t>40, 41</t>
+  </si>
+  <si>
+    <t>39, 41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>39, 40</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>id51-kazimir.png</t>
+  </si>
+  <si>
+    <t>id1-leonid.png</t>
+  </si>
+  <si>
+    <t>id2-elena.png</t>
+  </si>
+  <si>
+    <t>id32-vasilii.png</t>
+  </si>
+  <si>
+    <t>id11-milana.png</t>
+  </si>
+  <si>
+    <t>id5-maksim.png</t>
+  </si>
+  <si>
+    <t>id3-sergey.png</t>
+  </si>
+  <si>
+    <t>id6-sophia.png</t>
+  </si>
+  <si>
+    <t>id7-sviatik.png</t>
+  </si>
+  <si>
+    <t>id52-fedor.png</t>
+  </si>
+  <si>
+    <t>id31-sofia.png</t>
+  </si>
+  <si>
+    <t>id38-ivan.png</t>
+  </si>
+  <si>
+    <t>id35-nikolay.png</t>
+  </si>
+  <si>
+    <t>id33-fedor.png</t>
+  </si>
+  <si>
+    <t>id34-lelia.png</t>
+  </si>
+  <si>
+    <t>id29-lilina.png</t>
+  </si>
+  <si>
+    <t>Фотография Каземира сделана  в г. Ровны в 1928 году</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -501,7 +653,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -509,12 +661,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,62 +1001,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A72A30-50E6-4054-8331-253DB55A6B95}">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -918,8 +1091,11 @@
       <c r="J2">
         <v>28</v>
       </c>
-      <c r="K2">
-        <v>21</v>
+      <c r="K2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L2" t="s">
+        <v>146</v>
       </c>
       <c r="M2">
         <v>4</v>
@@ -934,7 +1110,7 @@
         <v>24</v>
       </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -942,19 +1118,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -963,19 +1139,25 @@
         <v>29</v>
       </c>
       <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
         <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
       </c>
       <c r="O3" t="s">
         <v>23</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>33</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -983,19 +1165,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1003,17 +1185,23 @@
       <c r="J4">
         <v>2</v>
       </c>
+      <c r="K4" t="s">
+        <v>147</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
       <c r="N4" t="s">
         <v>22</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="P4" t="s">
         <v>24</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1021,10 +1209,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
@@ -1033,7 +1221,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1041,14 +1229,20 @@
       <c r="J5">
         <v>2</v>
       </c>
+      <c r="K5" t="s">
+        <v>148</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
       <c r="N5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O5" t="s">
         <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1056,10 +1250,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
@@ -1068,7 +1262,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>6</v>
@@ -1079,17 +1273,26 @@
       <c r="J6">
         <v>2</v>
       </c>
+      <c r="K6" t="s">
+        <v>149</v>
+      </c>
+      <c r="L6" t="s">
+        <v>150</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
       <c r="N6" t="s">
         <v>22</v>
       </c>
       <c r="O6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P6" t="s">
         <v>24</v>
       </c>
       <c r="Q6" t="s">
-        <v>48</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1097,19 +1300,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -1120,17 +1323,26 @@
       <c r="J7">
         <v>11</v>
       </c>
+      <c r="K7" t="s">
+        <v>151</v>
+      </c>
+      <c r="L7" t="s">
+        <v>150</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
       <c r="N7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="O7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="Q7" t="s">
-        <v>54</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1138,10 +1350,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -1150,7 +1362,7 @@
         <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I8">
         <v>5</v>
@@ -1158,11 +1370,17 @@
       <c r="J8">
         <v>6</v>
       </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="O8" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1170,16 +1388,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H9">
         <v>9</v>
@@ -1190,8 +1408,17 @@
       <c r="J9">
         <v>11</v>
       </c>
+      <c r="K9" t="s">
+        <v>152</v>
+      </c>
+      <c r="L9" t="s">
+        <v>153</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
       <c r="O9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -1199,22 +1426,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H10">
         <v>8</v>
       </c>
+      <c r="L10" t="s">
+        <v>153</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
       <c r="O10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -1222,25 +1455,31 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11">
         <v>11</v>
       </c>
+      <c r="L11" t="s">
+        <v>154</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="P11" t="s">
         <v>24</v>
@@ -1251,28 +1490,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
+      <c r="L12" t="s">
+        <v>154</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
       <c r="O12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="Q12" t="s">
-        <v>72</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1280,16 +1525,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I13">
         <v>9</v>
@@ -1297,8 +1542,14 @@
       <c r="J13">
         <v>8</v>
       </c>
+      <c r="K13" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13">
+        <v>6</v>
+      </c>
       <c r="O13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1306,16 +1557,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I14">
         <v>9</v>
@@ -1323,8 +1574,14 @@
       <c r="J14">
         <v>8</v>
       </c>
+      <c r="K14" t="s">
+        <v>156</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
       <c r="O14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1332,19 +1589,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H15">
         <v>15</v>
@@ -1353,10 +1610,16 @@
         <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="L15" t="s">
+        <v>157</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
       </c>
       <c r="O15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1364,45 +1627,51 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H16">
         <v>14</v>
       </c>
+      <c r="L16" t="s">
+        <v>157</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
       <c r="O16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H17">
         <v>24</v>
@@ -1413,28 +1682,37 @@
       <c r="J17">
         <v>14</v>
       </c>
+      <c r="K17" t="s">
+        <v>158</v>
+      </c>
+      <c r="L17" t="s">
+        <v>159</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
       <c r="O17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I18">
         <v>15</v>
@@ -1442,28 +1720,34 @@
       <c r="J18">
         <v>14</v>
       </c>
+      <c r="K18" t="s">
+        <v>160</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
       <c r="O18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H19">
         <v>19</v>
@@ -1472,56 +1756,68 @@
         <v>29</v>
       </c>
       <c r="K19" t="s">
-        <v>92</v>
+        <v>86</v>
+      </c>
+      <c r="L19" t="s">
+        <v>161</v>
+      </c>
+      <c r="M19">
+        <v>4</v>
       </c>
       <c r="N19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H20">
         <v>18</v>
       </c>
+      <c r="L20" t="s">
+        <v>161</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
       <c r="O20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I21">
         <v>18</v>
@@ -1529,16 +1825,19 @@
       <c r="J21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -1547,50 +1846,62 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H22">
         <v>22</v>
       </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>162</v>
+      </c>
+      <c r="L22" t="s">
+        <v>163</v>
+      </c>
+      <c r="M22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>163</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I24">
         <v>21</v>
@@ -1598,51 +1909,60 @@
       <c r="J24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
         <v>20</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H25">
         <v>16</v>
       </c>
+      <c r="L25" t="s">
+        <v>159</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
       <c r="O25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I26">
         <v>24</v>
@@ -1650,28 +1970,34 @@
       <c r="J26">
         <v>16</v>
       </c>
+      <c r="K26" t="s">
+        <v>164</v>
+      </c>
+      <c r="M26">
+        <v>6</v>
+      </c>
       <c r="O26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I27">
         <v>24</v>
@@ -1680,21 +2006,24 @@
         <v>16</v>
       </c>
       <c r="K27" t="s">
-        <v>110</v>
+        <v>104</v>
+      </c>
+      <c r="M27">
+        <v>6</v>
       </c>
       <c r="O27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
         <v>19</v>
@@ -1703,7 +2032,7 @@
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G28">
         <v>2010</v>
@@ -1711,19 +2040,25 @@
       <c r="H28">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>162</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G29">
         <v>2019</v>
@@ -1731,25 +2066,31 @@
       <c r="H29">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>162</v>
+      </c>
+      <c r="M29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G30">
         <v>1995</v>
@@ -1764,55 +2105,73 @@
         <v>31</v>
       </c>
       <c r="K30" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="L30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H31">
         <v>29</v>
       </c>
       <c r="L31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H32">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L32" t="s">
+        <v>165</v>
+      </c>
+      <c r="M32">
+        <v>2</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H33">
         <v>31</v>
@@ -1820,16 +2179,25 @@
       <c r="I33">
         <v>51</v>
       </c>
-      <c r="K33">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>166</v>
+      </c>
+      <c r="L33" t="s">
+        <v>165</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H34">
         <v>36</v>
@@ -1841,18 +2209,27 @@
         <v>31</v>
       </c>
       <c r="K34" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="L34" t="s">
+        <v>167</v>
+      </c>
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H35">
         <v>38</v>
@@ -1864,15 +2241,24 @@
         <v>31</v>
       </c>
       <c r="K35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="L35" t="s">
+        <v>168</v>
+      </c>
+      <c r="M35">
+        <v>3</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H36">
         <v>44</v>
@@ -1884,26 +2270,41 @@
         <v>31</v>
       </c>
       <c r="K36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="L36" t="s">
+        <v>169</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H37">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>167</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H38">
         <v>53</v>
@@ -1914,30 +2315,45 @@
       <c r="J38">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>170</v>
+      </c>
+      <c r="M38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H39">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>168</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D40" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I40">
         <v>38</v>
@@ -1945,19 +2361,25 @@
       <c r="J40">
         <v>34</v>
       </c>
+      <c r="K40" t="s">
+        <v>171</v>
+      </c>
+      <c r="M40">
+        <v>4</v>
+      </c>
       <c r="O40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H41">
         <v>43</v>
@@ -1968,16 +2390,25 @@
       <c r="J41">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>172</v>
+      </c>
+      <c r="L41" t="s">
+        <v>173</v>
+      </c>
+      <c r="M41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D42" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I42">
         <v>38</v>
@@ -1985,16 +2416,22 @@
       <c r="J42">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>174</v>
+      </c>
+      <c r="M42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="C43" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D43" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="I43">
         <v>40</v>
@@ -2002,38 +2439,53 @@
       <c r="J43">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H44">
         <v>40</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L44" t="s">
+        <v>173</v>
+      </c>
+      <c r="M44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H45">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>169</v>
+      </c>
+      <c r="M45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H46">
         <v>48</v>
@@ -2044,13 +2496,22 @@
       <c r="J46">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>175</v>
+      </c>
+      <c r="L46" t="s">
+        <v>176</v>
+      </c>
+      <c r="M46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I47">
         <v>35</v>
@@ -2058,19 +2519,25 @@
       <c r="J47">
         <v>44</v>
       </c>
+      <c r="K47" t="s">
+        <v>177</v>
+      </c>
       <c r="L47" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="M47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D48" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I48">
         <v>48</v>
@@ -2078,103 +2545,139 @@
       <c r="J48">
         <v>45</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="C49" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" t="s">
         <v>134</v>
-      </c>
-      <c r="D49" t="s">
-        <v>140</v>
       </c>
       <c r="H49">
         <v>45</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L49" t="s">
+        <v>176</v>
+      </c>
+      <c r="M49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I50">
         <v>46</v>
       </c>
-      <c r="K50">
-        <v>50</v>
+      <c r="K50" t="s">
+        <v>178</v>
+      </c>
+      <c r="M50">
+        <v>5</v>
       </c>
       <c r="P50" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="I51">
         <v>46</v>
       </c>
-      <c r="K51">
-        <v>49</v>
+      <c r="K51" t="s">
+        <v>179</v>
+      </c>
+      <c r="M51">
+        <v>5</v>
       </c>
       <c r="O51" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="P51" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="L52" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="P52" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I53">
         <v>51</v>
       </c>
-      <c r="K53">
-        <v>32</v>
+      <c r="K53" t="s">
+        <v>180</v>
+      </c>
+      <c r="M53">
+        <v>2</v>
       </c>
       <c r="P53" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H54">
         <v>37</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L54" t="s">
+        <v>170</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I55">
         <v>37</v>
@@ -2182,16 +2685,19 @@
       <c r="J55">
         <v>53</v>
       </c>
-      <c r="K55">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>181</v>
+      </c>
+      <c r="M55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I56">
         <v>37</v>
@@ -2199,8 +2705,11 @@
       <c r="J56">
         <v>53</v>
       </c>
-      <c r="K56">
-        <v>54</v>
+      <c r="K56" t="s">
+        <v>182</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>